<commit_message>
Ray tune fixes now
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_lungs.xlsx
+++ b/configurations/experiment_configs_lungs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -215,10 +215,7 @@
     <t xml:space="preserve">samples_per_file</t>
   </si>
   <si>
-    <t xml:space="preserve">src_dims</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[192,192,128]</t>
+    <t xml:space="preserve">src_dim0</t>
   </si>
   <si>
     <t xml:space="preserve">[192,192,96]</t>
@@ -237,6 +234,9 @@
   </si>
   <si>
     <t xml:space="preserve">[256,256,128]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">src_dim1</t>
   </si>
   <si>
     <t xml:space="preserve">fgbg_ratio</t>
@@ -795,7 +795,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1114,13 +1114,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A4 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="31.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="44.88"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1199,34 +1203,62 @@
       <c r="A6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="n">
+        <v>192</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K6" s="2" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>69</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
@@ -1235,75 +1267,56 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>82</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1323,7 +1336,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1560,7 +1573,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1683,7 +1696,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1776,7 +1789,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1859,7 +1872,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2005,8 +2018,8 @@
   </sheetPr>
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
relative path fixes for HPC
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_lungs.xlsx
+++ b/configurations/experiment_configs_lungs.xlsx
@@ -485,7 +485,7 @@
     <t xml:space="preserve">remapping_lbd</t>
   </si>
   <si>
-    <t xml:space="preserve">/s/fran_storage/predictions/totalseg/LITS-1271</t>
+    <t xml:space="preserve">$cold_storage_folder/predictions/totalseg/LITS-1271</t>
   </si>
   <si>
     <t xml:space="preserve">TSL.label_localiser,TSL.lungs</t>
@@ -2022,7 +2022,7 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>